<commit_message>
time values (precision oone second)
</commit_message>
<xml_diff>
--- a/datetime.xlsx
+++ b/datetime.xlsx
@@ -135,15 +135,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="39.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
@@ -152,7 +153,7 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
@@ -189,6 +190,28 @@
         <v>0.550694444444444</v>
       </c>
       <c r="C4" s="2" t="n">
+        <v>25569</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>25569</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>0.999988425925926</v>
+      </c>
+      <c r="C6" s="2" t="n">
         <v>25569</v>
       </c>
     </row>

</xml_diff>